<commit_message>
Séparation du code & correction de l'UART. UART fonctionnel à 100% !
</commit_message>
<xml_diff>
--- a/ARTHUR/calculs excel.xlsx
+++ b/ARTHUR/calculs excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onion\Desktop\moql\Projet_ecole_MOQL\ARTHUR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artpe\Desktop\moql\Projet_ecole_MOQL\ARTHUR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1A1D8E-201F-4ADA-AAFC-B1CA87341075}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5695EA4C-9D97-4F3A-AD5E-35B999013A52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{38D826D1-AE61-4490-9D5B-7A9A335F935F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{38D826D1-AE61-4490-9D5B-7A9A335F935F}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc delai timer0 compA" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Frequence crystal</t>
   </si>
@@ -89,6 +91,9 @@
   </si>
   <si>
     <t>^-1</t>
+  </si>
+  <si>
+    <t>Prediv</t>
   </si>
 </sst>
 </file>
@@ -165,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -173,6 +178,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B74EE09A-6D33-4914-95A4-1D136E6F9F7E}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,37 +656,51 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>246</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1024</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>195</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
-        <v>65000</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="B6" s="1">
+        <v>80</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
-        <f>B2*B4*B5</f>
-        <v>0.99937499999999979</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B8" s="3">
+        <f>B2*B3*B5*B6</f>
+        <v>0.99839999999999995</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -694,7 +714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34187FAD-B14D-4B34-A100-482AD2642A98}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
AJout de l'init SPI/ commandes SPI (ajout commandes UART) git add ARTHUR! non testé
</commit_message>
<xml_diff>
--- a/ARTHUR/calculs excel.xlsx
+++ b/ARTHUR/calculs excel.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artpe\Desktop\moql\Projet_ecole_MOQL\ARTHUR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onion\Desktop\moql\Projet_ecole_MOQL\ARTHUR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5695EA4C-9D97-4F3A-AD5E-35B999013A52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCE1E83-01DA-47CE-B563-7015BAD277F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{38D826D1-AE61-4490-9D5B-7A9A335F935F}"/>
+    <workbookView xWindow="3405" yWindow="2985" windowWidth="20910" windowHeight="11835" activeTab="3" xr2:uid="{38D826D1-AE61-4490-9D5B-7A9A335F935F}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc delai timer0 compA" sheetId="1" r:id="rId1"/>
     <sheet name="Calc BAUD USART0" sheetId="2" r:id="rId2"/>
+    <sheet name="Commandes UART" sheetId="3" r:id="rId3"/>
+    <sheet name="Commandes SPI" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
   <si>
     <t>Frequence crystal</t>
   </si>
@@ -94,13 +94,184 @@
   </si>
   <si>
     <t>Prediv</t>
+  </si>
+  <si>
+    <t>SYSTEME:</t>
+  </si>
+  <si>
+    <t>MOTEUR:</t>
+  </si>
+  <si>
+    <t>FONCTIONNEMENT:</t>
+  </si>
+  <si>
+    <t>q/d -&gt; si tourne deja arret du robot</t>
+  </si>
+  <si>
+    <t>z/s -&gt; si avance/recule deja arret du robot</t>
+  </si>
+  <si>
+    <t>z|s puis q|d -&gt; avance/recule puis tourne</t>
+  </si>
+  <si>
+    <t>q|d puis z|s -&gt; tourne puis avance/recule</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>augmentation vitesse</t>
+  </si>
+  <si>
+    <t>etat du robot (ISP Capt_IR niveau batterie) =&gt; UART est forcement bon :D</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>diminuation vitesse</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>avance</t>
+  </si>
+  <si>
+    <t>tourne gauche</t>
+  </si>
+  <si>
+    <t>tourne droite</t>
+  </si>
+  <si>
+    <t>recule</t>
+  </si>
+  <si>
+    <t>UC1 UART BLUETOOTH</t>
+  </si>
+  <si>
+    <t>commutation heartbeat (cligno LED + envoie '*' UART) ON/OFF</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>SPI MASTER</t>
+  </si>
+  <si>
+    <t>0x01</t>
+  </si>
+  <si>
+    <t>SPI SLAVE</t>
+  </si>
+  <si>
+    <t>0x02</t>
+  </si>
+  <si>
+    <t>ACK</t>
+  </si>
+  <si>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>Demande mesure capt</t>
+  </si>
+  <si>
+    <t>Ping</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>Mesure capteur IR</t>
+  </si>
+  <si>
+    <t>0x08</t>
+  </si>
+  <si>
+    <t>Envoie donnée moteur</t>
+  </si>
+  <si>
+    <t>Angle moteur</t>
+  </si>
+  <si>
+    <t>0x09</t>
+  </si>
+  <si>
+    <t>Etat ?</t>
+  </si>
+  <si>
+    <t>0x05</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>NOK demande arret</t>
+  </si>
+  <si>
+    <t>0x0A</t>
+  </si>
+  <si>
+    <t>Balayage capteur</t>
+  </si>
+  <si>
+    <t>0x0B</t>
+  </si>
+  <si>
+    <t>Stop Balayage capteur</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>+ angle servo moteur</t>
+  </si>
+  <si>
+    <t>- angle servomoteur</t>
+  </si>
+  <si>
+    <t>0x0C</t>
+  </si>
+  <si>
+    <t>0x0D</t>
+  </si>
+  <si>
+    <t>Augmentation angle servo</t>
+  </si>
+  <si>
+    <t>Diminution angle servo</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>toggle balayage servo</t>
+  </si>
+  <si>
+    <t>0x06</t>
+  </si>
+  <si>
+    <t>Toggle balayage servo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,8 +293,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,8 +320,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -166,11 +350,244 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -179,6 +596,81 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,7 +1114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B74EE09A-6D33-4914-95A4-1D136E6F9F7E}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -793,4 +1285,415 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E59BF2-022A-4F9C-AE32-A8197C5DA150}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="42.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="14"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB46B1C-AEE3-473F-9152-CFBC5720BB8F}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="30"/>
+      <c r="B1" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="19"/>
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="30"/>
+      <c r="B2" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="30"/>
+      <c r="B3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="30"/>
+      <c r="B5" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="34"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="34"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="50"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="40"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="34"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="40"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="40"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="B12" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="40"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
+      <c r="B13" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="40"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="30">
+        <v>1</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="22"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="37"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="30">
+        <v>2</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="37"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="30"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="F5:G5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout de commande SPI, release du programme pour UC1 (SPI non testé mais fonctionne sur oscillo)
</commit_message>
<xml_diff>
--- a/ARTHUR/calculs excel.xlsx
+++ b/ARTHUR/calculs excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onion\Desktop\moql\Projet_ecole_MOQL\ARTHUR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artpe\Desktop\moql\Projet_ecole_MOQL\ARTHUR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCE1E83-01DA-47CE-B563-7015BAD277F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2CE0C8-5D92-43EF-9865-F016622B248A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="2985" windowWidth="20910" windowHeight="11835" activeTab="3" xr2:uid="{38D826D1-AE61-4490-9D5B-7A9A335F935F}"/>
+    <workbookView xWindow="4590" yWindow="0" windowWidth="14655" windowHeight="8325" firstSheet="1" activeTab="2" xr2:uid="{38D826D1-AE61-4490-9D5B-7A9A335F935F}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc delai timer0 compA" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
   <si>
     <t>Frequence crystal</t>
   </si>
@@ -265,6 +267,18 @@
   </si>
   <si>
     <t>Toggle balayage servo</t>
+  </si>
+  <si>
+    <t>0x0E</t>
+  </si>
+  <si>
+    <t>Get angle servo</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>commutateur empeche stop robot si detection obstacle</t>
   </si>
 </sst>
 </file>
@@ -327,7 +341,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -583,11 +597,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -597,56 +633,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -668,9 +671,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1289,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E59BF2-022A-4F9C-AE32-A8197C5DA150}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,139 +1343,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="43"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="12"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="14"/>
+      <c r="C3" s="40"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="14"/>
+      <c r="C4" s="40"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="11"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="13" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="11"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="34" t="s">
         <v>65</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="11"/>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="24"/>
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="53" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1448,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB46B1C-AEE3-473F-9152-CFBC5720BB8F}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1460,239 +1509,264 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30"/>
-      <c r="B1" s="18" t="s">
+      <c r="A1" s="22"/>
+      <c r="B1" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="19" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="20"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="25" t="s">
+      <c r="A2" s="22"/>
+      <c r="B2" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="27" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="12"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="22"/>
+      <c r="B3" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="42" t="s">
+      <c r="D3" s="48"/>
+      <c r="E3" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="22"/>
+      <c r="G3" s="48"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="31" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="28" t="s">
+      <c r="D5" s="45"/>
+      <c r="E5" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="34"/>
+      <c r="G5" s="45"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="28" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="34"/>
+      <c r="G6" s="45"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="38"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="45"/>
+      <c r="E8" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="37"/>
+      <c r="G8" s="38"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C10" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="13" t="s">
+      <c r="D10" s="46"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C11" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="40"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="13" t="s">
+      <c r="D11" s="45"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C12" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="40"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="40"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="13" t="s">
+      <c r="D12" s="45"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="29"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C14" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="13" t="s">
+      <c r="D14" s="45"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C15" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="40"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="30">
+      <c r="D15" s="45"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="29"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="22">
         <v>1</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C17" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="30">
+      <c r="D17" s="48"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="26"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="22">
         <v>2</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B18" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C18" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="37"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="30"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="24"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="26"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="22"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
+  <mergeCells count="16">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="F5:G5"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajour USI/SPI-slave sur Attiny85 encore en dev
</commit_message>
<xml_diff>
--- a/ARTHUR/calculs excel.xlsx
+++ b/ARTHUR/calculs excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artpe\Desktop\moql\Projet_ecole_MOQL\ARTHUR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2CE0C8-5D92-43EF-9865-F016622B248A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93640C0-CACE-494E-879B-7DC51C8726FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="0" windowWidth="14655" windowHeight="8325" firstSheet="1" activeTab="2" xr2:uid="{38D826D1-AE61-4490-9D5B-7A9A335F935F}"/>
+    <workbookView xWindow="4590" yWindow="0" windowWidth="14655" windowHeight="8325" firstSheet="1" activeTab="3" xr2:uid="{38D826D1-AE61-4490-9D5B-7A9A335F935F}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc delai timer0 compA" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="82">
   <si>
     <t>Frequence crystal</t>
   </si>
@@ -194,9 +194,6 @@
     <t>***</t>
   </si>
   <si>
-    <t>Mesure capteur IR</t>
-  </si>
-  <si>
     <t>0x08</t>
   </si>
   <si>
@@ -279,6 +276,12 @@
   </si>
   <si>
     <t>commutateur empeche stop robot si detection obstacle</t>
+  </si>
+  <si>
+    <t>Mesure capteur IR (first8bits)</t>
+  </si>
+  <si>
+    <t>Mesure capteur IR (Second 2bit)</t>
   </si>
 </sst>
 </file>
@@ -671,6 +674,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -687,21 +692,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -710,8 +703,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1332,7 +1335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E59BF2-022A-4F9C-AE32-A8197C5DA150}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -1343,11 +1346,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="43"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="45"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
@@ -1360,19 +1363,19 @@
       <c r="A3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="40"/>
+      <c r="C3" s="42"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="40"/>
+      <c r="C4" s="42"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
@@ -1452,37 +1455,37 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="33" t="s">
         <v>73</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>74</v>
       </c>
       <c r="C13" s="11"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="11"/>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" s="17"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="40" t="s">
         <v>79</v>
-      </c>
-      <c r="B16" s="53" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1497,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB46B1C-AEE3-473F-9152-CFBC5720BB8F}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1510,16 +1513,16 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22"/>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="42" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="42"/>
-      <c r="G1" s="43"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="22"/>
@@ -1531,7 +1534,7 @@
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>47</v>
@@ -1539,103 +1542,109 @@
       <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
+      <c r="A3" s="22">
+        <v>1</v>
+      </c>
       <c r="B3" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="48"/>
+      <c r="D3" s="47"/>
       <c r="E3" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="48"/>
+      <c r="F3" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="47"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="22">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
+      <c r="E4" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="47"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="44" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" s="45"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="45"/>
+      <c r="B6" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="51"/>
       <c r="E6" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="45"/>
+        <v>44</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="51"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="51"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
-      <c r="B8" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="20" t="s">
-        <v>51</v>
-      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="37"/>
       <c r="G8" s="38"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
+      <c r="B9" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="51"/>
+      <c r="E9" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="37"/>
+      <c r="G9" s="38"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" s="46"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="20"/>
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
@@ -1643,47 +1652,47 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+        <v>74</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="53"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="45"/>
+        <v>60</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="51"/>
       <c r="E12" s="27"/>
       <c r="F12" s="28"/>
       <c r="G12" s="29"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="38"/>
+      <c r="B13" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="51"/>
       <c r="E13" s="27"/>
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="45"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="38"/>
       <c r="E14" s="27"/>
       <c r="F14" s="28"/>
       <c r="G14" s="29"/>
@@ -1691,82 +1700,96 @@
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="B15" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="45"/>
+      <c r="D15" s="51"/>
       <c r="E15" s="27"/>
       <c r="F15" s="28"/>
       <c r="G15" s="29"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="11"/>
+      <c r="B16" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="51"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="29"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
-        <v>1</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="48"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="22">
-        <v>2</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="48"/>
+        <v>1</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="47"/>
       <c r="E18" s="24"/>
       <c r="F18" s="25"/>
       <c r="G18" s="26"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="17"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="22">
+        <v>2</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="47"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="22"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C8:D8"/>
+  <mergeCells count="17">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
-    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:D7"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tout les elements sont fonctionnels, quelques corrections à faire
</commit_message>
<xml_diff>
--- a/ARTHUR/calculs excel.xlsx
+++ b/ARTHUR/calculs excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artpe\Desktop\moql\Projet_ecole_MOQL\ARTHUR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93640C0-CACE-494E-879B-7DC51C8726FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8F956E-F515-4481-94FB-29C30BDEFF62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4590" yWindow="0" windowWidth="14655" windowHeight="8325" firstSheet="1" activeTab="3" xr2:uid="{38D826D1-AE61-4490-9D5B-7A9A335F935F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
   <si>
     <t>Frequence crystal</t>
   </si>
@@ -194,15 +194,9 @@
     <t>***</t>
   </si>
   <si>
-    <t>0x08</t>
-  </si>
-  <si>
     <t>Envoie donnée moteur</t>
   </si>
   <si>
-    <t>Angle moteur</t>
-  </si>
-  <si>
     <t>0x09</t>
   </si>
   <si>
@@ -282,6 +276,12 @@
   </si>
   <si>
     <t>Mesure capteur IR (Second 2bit)</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>0x10 + donnée</t>
   </si>
 </sst>
 </file>
@@ -691,17 +691,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -709,10 +706,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1455,37 +1455,37 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C13" s="11"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>66</v>
       </c>
       <c r="C14" s="11"/>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="36" t="s">
         <v>65</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>67</v>
       </c>
       <c r="C15" s="17"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1500,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB46B1C-AEE3-473F-9152-CFBC5720BB8F}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,7 +1511,7 @@
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22"/>
       <c r="B1" s="43" t="s">
         <v>43</v>
@@ -1524,7 +1524,7 @@
       <c r="F1" s="44"/>
       <c r="G1" s="45"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="22"/>
       <c r="B2" s="18" t="s">
         <v>44</v>
@@ -1534,50 +1534,59 @@
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>47</v>
       </c>
       <c r="G2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="22">
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="46" t="s">
         <v>49</v>
       </c>
       <c r="D3" s="47"/>
       <c r="E3" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="47"/>
+      <c r="H3" t="s">
         <v>80</v>
       </c>
-      <c r="G3" s="47"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="22">
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
       <c r="E4" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="52" t="s">
-        <v>81</v>
+      <c r="F4" s="46" t="s">
+        <v>79</v>
       </c>
       <c r="G4" s="47"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
       <c r="B5" s="32"/>
       <c r="C5" s="10"/>
@@ -1586,37 +1595,43 @@
       <c r="F5" s="10"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="51"/>
+      <c r="B6" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="50"/>
       <c r="E6" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="51"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="50"/>
+      <c r="H6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="51"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="50"/>
       <c r="E7" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" s="51"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="50"/>
+      <c r="H7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="37"/>
@@ -1625,22 +1640,22 @@
       <c r="F8" s="37"/>
       <c r="G8" s="38"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="51"/>
+        <v>74</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="50"/>
       <c r="E9" s="20" t="s">
         <v>51</v>
       </c>
       <c r="F9" s="37"/>
       <c r="G9" s="38"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="12"/>
       <c r="C10" s="10"/>
@@ -1649,46 +1664,55 @@
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="53"/>
+        <v>72</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="51"/>
       <c r="E11" s="20"/>
       <c r="F11" s="10"/>
       <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="51"/>
+        <v>58</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="50"/>
       <c r="E12" s="27"/>
       <c r="F12" s="28"/>
       <c r="G12" s="29"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="51"/>
+        <v>60</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="50"/>
       <c r="E13" s="27"/>
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="B14" s="12"/>
       <c r="C14" s="37"/>
@@ -1697,33 +1721,33 @@
       <c r="F14" s="28"/>
       <c r="G14" s="29"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="B15" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="50" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="51"/>
+      <c r="D15" s="50"/>
       <c r="E15" s="27"/>
       <c r="F15" s="28"/>
       <c r="G15" s="29"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="50" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="51"/>
+      <c r="D16" s="50"/>
       <c r="E16" s="27"/>
       <c r="F16" s="28"/>
       <c r="G16" s="29"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
       <c r="B17" s="12"/>
       <c r="C17" s="10"/>
@@ -1732,37 +1756,34 @@
       <c r="F17" s="10"/>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="22">
         <v>1</v>
       </c>
       <c r="B18" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="48" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" s="46" t="s">
-        <v>53</v>
       </c>
       <c r="D18" s="47"/>
       <c r="E18" s="24"/>
       <c r="F18" s="25"/>
       <c r="G18" s="26"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="22">
-        <v>2</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="46" t="s">
-        <v>54</v>
-      </c>
+      <c r="H18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="48"/>
       <c r="D19" s="47"/>
       <c r="E19" s="24"/>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
@@ -1773,6 +1794,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C9:D9"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="B1:D1"/>
@@ -1785,11 +1811,6 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="F4:G4"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout commentaire + modif excel
</commit_message>
<xml_diff>
--- a/ARTHUR/calculs excel.xlsx
+++ b/ARTHUR/calculs excel.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artpe\Desktop\moql\Projet_ecole_MOQL\ARTHUR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onion\Desktop\moql\Projet_ecole_MOQL\ARTHUR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8F956E-F515-4481-94FB-29C30BDEFF62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2951B7-063B-4296-84A7-91E50132912C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="0" windowWidth="14655" windowHeight="8325" firstSheet="1" activeTab="3" xr2:uid="{38D826D1-AE61-4490-9D5B-7A9A335F935F}"/>
+    <workbookView xWindow="4770" yWindow="2670" windowWidth="20910" windowHeight="11835" firstSheet="1" activeTab="3" xr2:uid="{38D826D1-AE61-4490-9D5B-7A9A335F935F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Calc delai timer0 compA" sheetId="1" r:id="rId1"/>
-    <sheet name="Calc BAUD USART0" sheetId="2" r:id="rId2"/>
-    <sheet name="Commandes UART" sheetId="3" r:id="rId3"/>
-    <sheet name="Commandes SPI" sheetId="4" r:id="rId4"/>
+    <sheet name="ATMEGA Calc delai timer0 compA" sheetId="1" r:id="rId1"/>
+    <sheet name="ATMEGA Calc BAUD USART0" sheetId="2" r:id="rId2"/>
+    <sheet name="ATMEGA Commandes UART" sheetId="3" r:id="rId3"/>
+    <sheet name="ATTINY timer1 PWM" sheetId="5" r:id="rId4"/>
+    <sheet name="Commandes SPI" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,9 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="97">
   <si>
     <t>Frequence crystal</t>
   </si>
@@ -185,9 +184,6 @@
     <t>0x04</t>
   </si>
   <si>
-    <t>Demande mesure capt</t>
-  </si>
-  <si>
     <t>Ping</t>
   </si>
   <si>
@@ -272,16 +268,64 @@
     <t>commutateur empeche stop robot si detection obstacle</t>
   </si>
   <si>
-    <t>Mesure capteur IR (first8bits)</t>
-  </si>
-  <si>
     <t>Mesure capteur IR (Second 2bit)</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>0x10 + donnée</t>
+  </si>
+  <si>
+    <t>Ordre</t>
+  </si>
+  <si>
+    <t>Demande mesure capt (1/2)</t>
+  </si>
+  <si>
+    <t>Demande mesure capt (2/2)</t>
+  </si>
+  <si>
+    <t>Mesure capteur IR (first 8bits)</t>
+  </si>
+  <si>
+    <t>Angle (8-16) du servo en cours</t>
+  </si>
+  <si>
+    <t>Active ou desactive le balayage du servomoteur</t>
+  </si>
+  <si>
+    <t>Active balayage</t>
+  </si>
+  <si>
+    <t>Desactive balayage</t>
+  </si>
+  <si>
+    <t>Augmente l'angle du servo</t>
+  </si>
+  <si>
+    <t>Diminue l'angle du servo</t>
+  </si>
+  <si>
+    <t>Permet de controller le servo avec le master</t>
+  </si>
+  <si>
+    <t>Rapport d'etat si obstacle</t>
+  </si>
+  <si>
+    <t>Mesure en 10 bits</t>
+  </si>
+  <si>
+    <t>Heartbeat du slave (verification prblème liaison spi)</t>
+  </si>
+  <si>
+    <t>OCR0B</t>
+  </si>
+  <si>
+    <t>1ms</t>
+  </si>
+  <si>
+    <t>2ms</t>
+  </si>
+  <si>
+    <t>VALEUR OCR1B</t>
   </si>
 </sst>
 </file>
@@ -318,7 +362,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,8 +387,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -525,7 +581,119 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -537,26 +705,9 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <right/>
+      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -566,67 +717,17 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -640,31 +741,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
@@ -674,8 +755,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -691,25 +843,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1159,7 +1317,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,7 +1494,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,14 +1504,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="10"/>
@@ -1363,19 +1521,19 @@
       <c r="A3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="42"/>
+      <c r="C3" s="57"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="57"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
@@ -1389,23 +1547,23 @@
       <c r="B6" s="10"/>
       <c r="C6" s="11"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="17" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="11"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="46" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1416,7 +1574,7 @@
       <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1427,7 +1585,7 @@
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1438,55 +1596,56 @@
       <c r="B11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="33" t="s">
-        <v>71</v>
-      </c>
       <c r="C13" s="11"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="11"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B15" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="11"/>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="17"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="40" t="s">
-        <v>77</v>
-      </c>
+      <c r="C16" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1499,310 +1658,420 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB46B1C-AEE3-473F-9152-CFBC5720BB8F}">
-  <dimension ref="A1:H20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CC8AB4-06CE-4E91-A7D7-AC96F992C9D7}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <f>1*10^6</f>
+        <v>1000000</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <f>1/B1</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2">
+        <v>128</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3">
+        <f>0.02</f>
+        <v>0.02</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="1">
+        <f>B4/(B2*B3)</f>
+        <v>156.25</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="55"/>
+      <c r="C9" s="53"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="51">
+        <f>0.001/(B2*B3)</f>
+        <v>7.8125000000000009</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="1">
+        <f>0.002/(B2*B3)</f>
+        <v>15.625000000000002</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB46B1C-AEE3-473F-9152-CFBC5720BB8F}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" style="23" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="23" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="23"/>
+    <col min="4" max="4" width="20" style="23" customWidth="1"/>
+    <col min="5" max="6" width="11.42578125" style="23"/>
+    <col min="7" max="7" width="18.7109375" style="23" customWidth="1"/>
+    <col min="8" max="8" width="68.42578125" style="23" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22"/>
-      <c r="B1" s="43" t="s">
+      <c r="A1" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="44" t="s">
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="45"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="66"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="39"/>
+      <c r="B2" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="22"/>
+      <c r="H2" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="39">
+        <v>1</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="62"/>
+      <c r="E3" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="19" t="s">
+      <c r="F3" s="62" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="63"/>
+      <c r="H3" s="61" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="39">
+        <v>2</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="62"/>
+      <c r="E4" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="63"/>
+      <c r="H4" s="61"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="39"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="39"/>
+      <c r="B6" s="69" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="62"/>
+      <c r="E6" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+      <c r="G6" s="63"/>
+      <c r="H6" s="61" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="39"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="63"/>
+      <c r="H7" s="61"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="39"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="22"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="39"/>
+      <c r="B9" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="62"/>
+      <c r="E9" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="63"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="39"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="39"/>
+      <c r="B11" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="68"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="39"/>
+      <c r="B12" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="62"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="39"/>
+      <c r="B13" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="67" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="62"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="39"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="32"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="39"/>
+      <c r="B15" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="62"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="39"/>
+      <c r="B16" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="62"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="39"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="22"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="39">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="31" t="s">
+      <c r="B18" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="47"/>
-      <c r="H3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="22">
-        <v>2</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="46" t="s">
-        <v>79</v>
-      </c>
-      <c r="G4" s="47"/>
-      <c r="H4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="50"/>
-      <c r="H6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="53"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" s="50"/>
-      <c r="H7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="37"/>
-      <c r="G9" s="38"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="51"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
-      <c r="H11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="29"/>
-      <c r="H12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="29"/>
-      <c r="H13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="50"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="29"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="29"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="22">
-        <v>1</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C18" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="47"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="26"/>
-      <c r="H18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="22"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="17"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="39"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
+  <mergeCells count="20">
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="C12:D12"/>
@@ -1810,7 +2079,19 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
     <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B6:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>